<commit_message>
Fix BOM and CPL
</commit_message>
<xml_diff>
--- a/001-‘’Cheese‘’/002-BOM_BMI160_160_2023-06-16.xlsx
+++ b/001-‘’Cheese‘’/002-BOM_BMI160_160_2023-06-16.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170682A-C142-4A17-B3F3-B9F1BA478600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="8630" yWindow="840" windowWidth="14970" windowHeight="13030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="BOM_BMI160_160_2023-06-16" state="visible" r:id="rId4"/>
+    <sheet name="BOM_BMI160_160_2023-06-16" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
   <si>
     <t>No.</t>
   </si>
@@ -46,19 +50,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>HDR-M-2.54_1x2</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>HDR-M-2.54_1X2</t>
-  </si>
-  <si>
     <t/>
-  </si>
-  <si>
-    <t>C124375</t>
   </si>
   <si>
     <t>LCSC</t>
@@ -394,14 +386,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -428,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -764,12 +763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
@@ -806,686 +807,656 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="I7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>45</v>
-      </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="I9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" t="s">
-        <v>55</v>
-      </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="I10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" t="s">
-        <v>61</v>
-      </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="I11" t="s">
         <v>63</v>
       </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" t="s">
-        <v>67</v>
-      </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="I12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" t="s">
-        <v>73</v>
-      </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
         <v>74</v>
       </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="I13" t="s">
         <v>75</v>
       </c>
-      <c r="D13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" t="s">
-        <v>79</v>
-      </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
         <v>77</v>
       </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" t="s">
-        <v>81</v>
-      </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" t="s">
         <v>84</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" t="s">
-        <v>88</v>
-      </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" t="s">
-        <v>78</v>
-      </c>
-      <c r="I16" t="s">
-        <v>93</v>
-      </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" t="s">
         <v>98</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="I18" t="s">
         <v>99</v>
       </c>
-      <c r="D18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18" t="s">
-        <v>102</v>
-      </c>
-      <c r="I18" t="s">
-        <v>103</v>
-      </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="I19" t="s">
         <v>105</v>
       </c>
-      <c r="D19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19" t="s">
-        <v>108</v>
-      </c>
-      <c r="I19" t="s">
-        <v>109</v>
-      </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
         <v>110</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="I20" t="s">
         <v>111</v>
       </c>
-      <c r="D20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" t="s">
-        <v>111</v>
-      </c>
-      <c r="H20" t="s">
-        <v>114</v>
-      </c>
-      <c r="I20" t="s">
-        <v>115</v>
-      </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" t="s">
         <v>116</v>
       </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" t="s">
-        <v>120</v>
-      </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" t="s">
         <v>121</v>
       </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" t="s">
-        <v>125</v>
-      </c>
       <c r="J22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>